<commit_message>
correção no codigo. estável
</commit_message>
<xml_diff>
--- a/vol_carteira_21-9-2021.xlsx
+++ b/vol_carteira_21-9-2021.xlsx
@@ -416,7 +416,7 @@
         <v>43874</v>
       </c>
       <c r="B3">
-        <v>0.0158014378466392</v>
+        <v>0.017019691470072</v>
       </c>
       <c r="C3">
         <v>0.01203573968630153</v>
@@ -427,7 +427,7 @@
         <v>43875</v>
       </c>
       <c r="B4">
-        <v>0.01550812736194737</v>
+        <v>0.01671488664484773</v>
       </c>
       <c r="C4">
         <v>0.01199565219408701</v>
@@ -438,7 +438,7 @@
         <v>43878</v>
       </c>
       <c r="B5">
-        <v>0.01518244275446247</v>
+        <v>0.01635848054204328</v>
       </c>
       <c r="C5">
         <v>0.01183084714850297</v>
@@ -449,7 +449,7 @@
         <v>43879</v>
       </c>
       <c r="B6">
-        <v>0.01476107690601528</v>
+        <v>0.01592746973744544</v>
       </c>
       <c r="C6">
         <v>0.01155085537236041</v>
@@ -460,7 +460,7 @@
         <v>43880</v>
       </c>
       <c r="B7">
-        <v>0.01458838027985448</v>
+        <v>0.01575763125361396</v>
       </c>
       <c r="C7">
         <v>0.0116237739713944</v>
@@ -471,7 +471,7 @@
         <v>43881</v>
       </c>
       <c r="B8">
-        <v>0.01445516323294744</v>
+        <v>0.01559612709236261</v>
       </c>
       <c r="C8">
         <v>0.01194935386744394</v>
@@ -482,7 +482,7 @@
         <v>43882</v>
       </c>
       <c r="B9">
-        <v>0.01419810192473082</v>
+        <v>0.01530196026754339</v>
       </c>
       <c r="C9">
         <v>0.01176918233058362</v>
@@ -493,7 +493,7 @@
         <v>43888</v>
       </c>
       <c r="B10">
-        <v>0.02317703690910367</v>
+        <v>0.02468699209400041</v>
       </c>
       <c r="C10">
         <v>0.02429647415923554</v>
@@ -504,7 +504,7 @@
         <v>43889</v>
       </c>
       <c r="B11">
-        <v>0.02261410480744308</v>
+        <v>0.02411588473289977</v>
       </c>
       <c r="C11">
         <v>0.02396712384079856</v>
@@ -515,7 +515,7 @@
         <v>43892</v>
       </c>
       <c r="B12">
-        <v>0.02418283631206349</v>
+        <v>0.02575904370690595</v>
       </c>
       <c r="C12">
         <v>0.02413823437917088</v>
@@ -526,7 +526,7 @@
         <v>43893</v>
       </c>
       <c r="B13">
-        <v>0.02685372327795814</v>
+        <v>0.02866611397801576</v>
       </c>
       <c r="C13">
         <v>0.02357693253502759</v>
@@ -537,7 +537,7 @@
         <v>43894</v>
       </c>
       <c r="B14">
-        <v>0.02677657987274158</v>
+        <v>0.02858480923098559</v>
       </c>
       <c r="C14">
         <v>0.02336697573690455</v>
@@ -548,7 +548,7 @@
         <v>43895</v>
       </c>
       <c r="B15">
-        <v>0.02722294790272932</v>
+        <v>0.02886062823844144</v>
       </c>
       <c r="C15">
         <v>0.02480265956370888</v>
@@ -559,7 +559,7 @@
         <v>43896</v>
       </c>
       <c r="B16">
-        <v>0.03235645491183113</v>
+        <v>0.03413274635699948</v>
       </c>
       <c r="C16">
         <v>0.0255161659665899</v>
@@ -570,7 +570,7 @@
         <v>43899</v>
       </c>
       <c r="B17">
-        <v>0.04327552289853066</v>
+        <v>0.04486614055743004</v>
       </c>
       <c r="C17">
         <v>0.03658014497248158</v>
@@ -581,7 +581,7 @@
         <v>43900</v>
       </c>
       <c r="B18">
-        <v>0.04418495986822023</v>
+        <v>0.04585207898733967</v>
       </c>
       <c r="C18">
         <v>0.03986941728503648</v>
@@ -592,7 +592,7 @@
         <v>43901</v>
       </c>
       <c r="B19">
-        <v>0.04797284892423637</v>
+        <v>0.04967699142939014</v>
       </c>
       <c r="C19">
         <v>0.04180025937352916</v>
@@ -603,7 +603,7 @@
         <v>43902</v>
       </c>
       <c r="B20">
-        <v>0.05931712232738139</v>
+        <v>0.0609791345799774</v>
       </c>
       <c r="C20">
         <v>0.05191175769773176</v>
@@ -614,7 +614,7 @@
         <v>43903</v>
       </c>
       <c r="B21">
-        <v>0.06260496984725324</v>
+        <v>0.06450669316268109</v>
       </c>
       <c r="C21">
         <v>0.06023106351232612</v>
@@ -625,7 +625,7 @@
         <v>43906</v>
       </c>
       <c r="B22">
-        <v>0.07299882898249814</v>
+        <v>0.07509457241627016</v>
       </c>
       <c r="C22">
         <v>0.06593254674355932</v>
@@ -636,7 +636,7 @@
         <v>43907</v>
       </c>
       <c r="B23">
-        <v>0.07453064501316058</v>
+        <v>0.07656123176457488</v>
       </c>
       <c r="C23">
         <v>0.06587319570321046</v>
@@ -647,7 +647,7 @@
         <v>43908</v>
       </c>
       <c r="B24">
-        <v>0.07250692392720635</v>
+        <v>0.0759707028808647</v>
       </c>
       <c r="C24">
         <v>0.06735972509134358</v>
@@ -658,7 +658,7 @@
         <v>43909</v>
       </c>
       <c r="B25">
-        <v>0.07829615218199303</v>
+        <v>0.08177571520833356</v>
       </c>
       <c r="C25">
         <v>0.06628014481487397</v>
@@ -669,7 +669,7 @@
         <v>43910</v>
       </c>
       <c r="B26">
-        <v>0.07646307926455673</v>
+        <v>0.07991623523180018</v>
       </c>
       <c r="C26">
         <v>0.06460192639314694</v>
@@ -680,7 +680,7 @@
         <v>43913</v>
       </c>
       <c r="B27">
-        <v>0.07469589647722778</v>
+        <v>0.07798531575880378</v>
       </c>
       <c r="C27">
         <v>0.06343194843280568</v>
@@ -691,7 +691,7 @@
         <v>43914</v>
       </c>
       <c r="B28">
-        <v>0.0757045513939904</v>
+        <v>0.07915311463127503</v>
       </c>
       <c r="C28">
         <v>0.06651897264449028</v>
@@ -702,7 +702,7 @@
         <v>43915</v>
       </c>
       <c r="B29">
-        <v>0.07551608930394711</v>
+        <v>0.07896436421709076</v>
       </c>
       <c r="C29">
         <v>0.06753756994762387</v>
@@ -713,7 +713,7 @@
         <v>43916</v>
       </c>
       <c r="B30">
-        <v>0.07371444940892531</v>
+        <v>0.07708503779585529</v>
       </c>
       <c r="C30">
         <v>0.06659468370971079</v>
@@ -724,7 +724,7 @@
         <v>43917</v>
       </c>
       <c r="B31">
-        <v>0.07284648907002117</v>
+        <v>0.07610971291352933</v>
       </c>
       <c r="C31">
         <v>0.06577450604540606</v>
@@ -735,7 +735,7 @@
         <v>43920</v>
       </c>
       <c r="B32">
-        <v>0.07095535841570393</v>
+        <v>0.0742116361881639</v>
       </c>
       <c r="C32">
         <v>0.06437164573875026</v>
@@ -746,7 +746,7 @@
         <v>43921</v>
       </c>
       <c r="B33">
-        <v>0.0701516580161719</v>
+        <v>0.07337063344522954</v>
       </c>
       <c r="C33">
         <v>0.06280548823344138</v>
@@ -757,7 +757,7 @@
         <v>43922</v>
       </c>
       <c r="B34">
-        <v>0.06909830815538533</v>
+        <v>0.07223623114764617</v>
       </c>
       <c r="C34">
         <v>0.06135377694291873</v>
@@ -768,7 +768,7 @@
         <v>43923</v>
       </c>
       <c r="B35">
-        <v>0.06830986584229126</v>
+        <v>0.07149600057781971</v>
       </c>
       <c r="C35">
         <v>0.06012230443966886</v>
@@ -779,7 +779,7 @@
         <v>43924</v>
       </c>
       <c r="B36">
-        <v>0.06714051891589137</v>
+        <v>0.07041932164192609</v>
       </c>
       <c r="C36">
         <v>0.05894384615991978</v>
@@ -790,7 +790,7 @@
         <v>43927</v>
       </c>
       <c r="B37">
-        <v>0.07225070274128431</v>
+        <v>0.07557229977320595</v>
       </c>
       <c r="C37">
         <v>0.05965839285419682</v>
@@ -801,7 +801,7 @@
         <v>43928</v>
       </c>
       <c r="B38">
-        <v>0.0702773174243351</v>
+        <v>0.07364684879447006</v>
       </c>
       <c r="C38">
         <v>0.05871275952641448</v>
@@ -812,7 +812,7 @@
         <v>43929</v>
       </c>
       <c r="B39">
-        <v>0.06657406409487217</v>
+        <v>0.07139325480178214</v>
       </c>
       <c r="C39">
         <v>0.0577121108125928</v>
@@ -823,7 +823,7 @@
         <v>43930</v>
       </c>
       <c r="B40">
-        <v>0.06535876394680884</v>
+        <v>0.06999428481156912</v>
       </c>
       <c r="C40">
         <v>0.05628308820460075</v>
@@ -834,7 +834,7 @@
         <v>43934</v>
       </c>
       <c r="B41">
-        <v>0.0636548134792484</v>
+        <v>0.06822673326799217</v>
       </c>
       <c r="C41">
         <v>0.05500601249235533</v>
@@ -845,7 +845,7 @@
         <v>43935</v>
       </c>
       <c r="B42">
-        <v>0.06300997257439395</v>
+        <v>0.06741795640912561</v>
       </c>
       <c r="C42">
         <v>0.05373317871038735</v>
@@ -856,7 +856,7 @@
         <v>43936</v>
       </c>
       <c r="B43">
-        <v>0.06154785424118246</v>
+        <v>0.06578100398600119</v>
       </c>
       <c r="C43">
         <v>0.0524345052120358</v>
@@ -867,7 +867,7 @@
         <v>43937</v>
       </c>
       <c r="B44">
-        <v>0.06023077401234313</v>
+        <v>0.06425878386988979</v>
       </c>
       <c r="C44">
         <v>0.0511572327812047</v>
@@ -878,7 +878,7 @@
         <v>43938</v>
       </c>
       <c r="B45">
-        <v>0.05866707678809418</v>
+        <v>0.06268707088021695</v>
       </c>
       <c r="C45">
         <v>0.05001840210606343</v>
@@ -889,7 +889,7 @@
         <v>43941</v>
       </c>
       <c r="B46">
-        <v>0.05741250723107099</v>
+        <v>0.06123132502138908</v>
       </c>
       <c r="C46">
         <v>0.04875384216844891</v>
@@ -900,7 +900,7 @@
         <v>43943</v>
       </c>
       <c r="B47">
-        <v>0.05629688416424847</v>
+        <v>0.06007895610360133</v>
       </c>
       <c r="C47">
         <v>0.04779644731011091</v>
@@ -911,7 +911,7 @@
         <v>43944</v>
       </c>
       <c r="B48">
-        <v>0.05484313696520669</v>
+        <v>0.05855633146977006</v>
       </c>
       <c r="C48">
         <v>0.04665615759061403</v>
@@ -922,7 +922,7 @@
         <v>43945</v>
       </c>
       <c r="B49">
-        <v>0.05449923990234202</v>
+        <v>0.05813175717102496</v>
       </c>
       <c r="C49">
         <v>0.04700178456870435</v>
@@ -933,7 +933,7 @@
         <v>43948</v>
       </c>
       <c r="B50">
-        <v>0.05650465453757218</v>
+        <v>0.06008807856478512</v>
       </c>
       <c r="C50">
         <v>0.04672226666144033</v>
@@ -944,7 +944,7 @@
         <v>43949</v>
       </c>
       <c r="B51">
-        <v>0.05502202528052941</v>
+        <v>0.05867854301814598</v>
       </c>
       <c r="C51">
         <v>0.04639346376780736</v>
@@ -955,7 +955,7 @@
         <v>43950</v>
       </c>
       <c r="B52">
-        <v>0.05366647451798232</v>
+        <v>0.057333557475228</v>
       </c>
       <c r="C52">
         <v>0.04548877118412507</v>
@@ -966,7 +966,7 @@
         <v>43951</v>
       </c>
       <c r="B53">
-        <v>0.0529461002314414</v>
+        <v>0.05666641477826202</v>
       </c>
       <c r="C53">
         <v>0.04493765078840034</v>
@@ -977,7 +977,7 @@
         <v>43955</v>
       </c>
       <c r="B54">
-        <v>0.05248373412672819</v>
+        <v>0.05618304248594055</v>
       </c>
       <c r="C54">
         <v>0.04401203484271313</v>
@@ -988,7 +988,7 @@
         <v>43956</v>
       </c>
       <c r="B55">
-        <v>0.05109823012254426</v>
+        <v>0.05478325395736375</v>
       </c>
       <c r="C55">
         <v>0.04294397880004152</v>
@@ -999,7 +999,7 @@
         <v>43957</v>
       </c>
       <c r="B56">
-        <v>0.04999240807798028</v>
+        <v>0.0535375517171014</v>
       </c>
       <c r="C56">
         <v>0.04186548638432346</v>
@@ -1010,7 +1010,7 @@
         <v>43958</v>
       </c>
       <c r="B57">
-        <v>0.04876147196480075</v>
+        <v>0.05221598392899911</v>
       </c>
       <c r="C57">
         <v>0.04087135139955405</v>
@@ -1021,7 +1021,7 @@
         <v>43959</v>
       </c>
       <c r="B58">
-        <v>0.04778212553631846</v>
+        <v>0.05124853666646857</v>
       </c>
       <c r="C58">
         <v>0.04033424095686056</v>
@@ -1032,7 +1032,7 @@
         <v>43962</v>
       </c>
       <c r="B59">
-        <v>0.04752376732409833</v>
+        <v>0.05253139004972127</v>
       </c>
       <c r="C59">
         <v>0.03944113141349114</v>
@@ -1043,7 +1043,7 @@
         <v>43963</v>
       </c>
       <c r="B60">
-        <v>0.04672819738049888</v>
+        <v>0.05157201606222137</v>
       </c>
       <c r="C60">
         <v>0.03856360738921873</v>
@@ -1054,7 +1054,7 @@
         <v>43964</v>
       </c>
       <c r="B61">
-        <v>0.04748846093814904</v>
+        <v>0.05230932061420943</v>
       </c>
       <c r="C61">
         <v>0.03758738648672391</v>
@@ -1065,7 +1065,7 @@
         <v>43965</v>
       </c>
       <c r="B62">
-        <v>0.04635252368066232</v>
+        <v>0.05104656072614788</v>
       </c>
       <c r="C62">
         <v>0.03683740565548518</v>
@@ -1076,7 +1076,7 @@
         <v>43966</v>
       </c>
       <c r="B63">
-        <v>0.04533970723319829</v>
+        <v>0.04991230834185112</v>
       </c>
       <c r="C63">
         <v>0.03610891534315316</v>
@@ -1087,7 +1087,7 @@
         <v>43969</v>
       </c>
       <c r="B64">
-        <v>0.04597318505578026</v>
+        <v>0.0505866927033464</v>
       </c>
       <c r="C64">
         <v>0.03669697768399039</v>
@@ -1098,7 +1098,7 @@
         <v>43970</v>
       </c>
       <c r="B65">
-        <v>0.04483001951063287</v>
+        <v>0.04932362785528679</v>
       </c>
       <c r="C65">
         <v>0.03579257100808601</v>
@@ -1109,7 +1109,7 @@
         <v>43971</v>
       </c>
       <c r="B66">
-        <v>0.04401810125696648</v>
+        <v>0.04838930324722594</v>
       </c>
       <c r="C66">
         <v>0.03491866683236996</v>
@@ -1120,7 +1120,7 @@
         <v>43972</v>
       </c>
       <c r="B67">
-        <v>0.0431404496267566</v>
+        <v>0.04738559017372812</v>
       </c>
       <c r="C67">
         <v>0.03431859659537128</v>
@@ -1131,7 +1131,7 @@
         <v>43973</v>
       </c>
       <c r="B68">
-        <v>0.04228892199660608</v>
+        <v>0.04647729614293922</v>
       </c>
       <c r="C68">
         <v>0.03355031525888069</v>
@@ -1142,7 +1142,7 @@
         <v>43976</v>
       </c>
       <c r="B69">
-        <v>0.04175660709111539</v>
+        <v>0.04583670248082902</v>
       </c>
       <c r="C69">
         <v>0.03387751197804082</v>
@@ -1153,7 +1153,7 @@
         <v>43977</v>
       </c>
       <c r="B70">
-        <v>0.04074252028830105</v>
+        <v>0.0447627468711294</v>
       </c>
       <c r="C70">
         <v>0.03303976076249297</v>
@@ -1164,7 +1164,7 @@
         <v>43978</v>
       </c>
       <c r="B71">
-        <v>0.03995751923439331</v>
+        <v>0.04382772067293706</v>
       </c>
       <c r="C71">
         <v>0.03269116857399281</v>
@@ -1175,7 +1175,7 @@
         <v>43979</v>
       </c>
       <c r="B72">
-        <v>0.03900062975334515</v>
+        <v>0.04278300636951005</v>
       </c>
       <c r="C72">
         <v>0.03204063317522624</v>
@@ -1186,7 +1186,7 @@
         <v>43980</v>
       </c>
       <c r="B73">
-        <v>0.03827501872909173</v>
+        <v>0.04194058944270251</v>
       </c>
       <c r="C73">
         <v>0.03123220855731669</v>
@@ -1197,7 +1197,7 @@
         <v>43983</v>
       </c>
       <c r="B74">
-        <v>0.03729236566389127</v>
+        <v>0.04090165402460886</v>
       </c>
       <c r="C74">
         <v>0.03052668518326686</v>
@@ -1208,7 +1208,7 @@
         <v>43984</v>
       </c>
       <c r="B75">
-        <v>0.03717215913253748</v>
+        <v>0.04070940424480148</v>
       </c>
       <c r="C75">
         <v>0.03017736830038884</v>
@@ -1219,7 +1219,7 @@
         <v>43985</v>
       </c>
       <c r="B76">
-        <v>0.03652686663221691</v>
+        <v>0.03993152001208172</v>
       </c>
       <c r="C76">
         <v>0.02962472910718282</v>
@@ -1230,7 +1230,7 @@
         <v>43986</v>
       </c>
       <c r="B77">
-        <v>0.03586019875464506</v>
+        <v>0.03913914446019827</v>
       </c>
       <c r="C77">
         <v>0.02888200831923083</v>
@@ -1241,7 +1241,7 @@
         <v>43987</v>
       </c>
       <c r="B78">
-        <v>0.03625167696494735</v>
+        <v>0.03900369052278187</v>
       </c>
       <c r="C78">
         <v>0.02815627176798667</v>
@@ -1252,7 +1252,7 @@
         <v>43990</v>
       </c>
       <c r="B79">
-        <v>0.03540715146729766</v>
+        <v>0.03810328265571431</v>
       </c>
       <c r="C79">
         <v>0.02798568117693911</v>
@@ -1263,7 +1263,7 @@
         <v>43991</v>
       </c>
       <c r="B80">
-        <v>0.03529779750725293</v>
+        <v>0.03803144409853825</v>
       </c>
       <c r="C80">
         <v>0.02751680904048492</v>
@@ -1274,7 +1274,7 @@
         <v>43992</v>
       </c>
       <c r="B81">
-        <v>0.03469896603179248</v>
+        <v>0.03737011634979694</v>
       </c>
       <c r="C81">
         <v>0.02751004243766103</v>
@@ -1285,7 +1285,7 @@
         <v>43994</v>
       </c>
       <c r="B82">
-        <v>0.03496180045139823</v>
+        <v>0.03757439907620498</v>
       </c>
       <c r="C82">
         <v>0.02737579425992976</v>
@@ -1296,7 +1296,7 @@
         <v>43997</v>
       </c>
       <c r="B83">
-        <v>0.03420538859373647</v>
+        <v>0.03670440546366842</v>
       </c>
       <c r="C83">
         <v>0.02674556139089383</v>
@@ -1307,7 +1307,7 @@
         <v>43998</v>
       </c>
       <c r="B84">
-        <v>0.03390411281792417</v>
+        <v>0.03635932412187325</v>
       </c>
       <c r="C84">
         <v>0.02614135792736564</v>
@@ -1318,7 +1318,7 @@
         <v>43999</v>
       </c>
       <c r="B85">
-        <v>0.03305622343718821</v>
+        <v>0.03546005116744032</v>
       </c>
       <c r="C85">
         <v>0.02576042400929134</v>
@@ -1329,7 +1329,7 @@
         <v>44000</v>
       </c>
       <c r="B86">
-        <v>0.03226626658276681</v>
+        <v>0.03459092371154633</v>
       </c>
       <c r="C86">
         <v>0.025109622038828</v>
@@ -1340,7 +1340,7 @@
         <v>44001</v>
       </c>
       <c r="B87">
-        <v>0.03148193978916444</v>
+        <v>0.03376430164147674</v>
       </c>
       <c r="C87">
         <v>0.02447387452854881</v>
@@ -1351,7 +1351,7 @@
         <v>44004</v>
       </c>
       <c r="B88">
-        <v>0.03114009299681486</v>
+        <v>0.03339379031645383</v>
       </c>
       <c r="C88">
         <v>0.02416475755864713</v>
@@ -1362,7 +1362,7 @@
         <v>44005</v>
       </c>
       <c r="B89">
-        <v>0.03085709261184756</v>
+        <v>0.03305284108471843</v>
       </c>
       <c r="C89">
         <v>0.02356039750602298</v>
@@ -1373,7 +1373,7 @@
         <v>44006</v>
       </c>
       <c r="B90">
-        <v>0.03065790473396683</v>
+        <v>0.03285945830681831</v>
       </c>
       <c r="C90">
         <v>0.0234103339647076</v>
@@ -1384,7 +1384,7 @@
         <v>44007</v>
       </c>
       <c r="B91">
-        <v>0.03012342641749507</v>
+        <v>0.03225886654153358</v>
       </c>
       <c r="C91">
         <v>0.02301577671618134</v>
@@ -1395,7 +1395,7 @@
         <v>44008</v>
       </c>
       <c r="B92">
-        <v>0.029985809445549</v>
+        <v>0.03211338967909708</v>
       </c>
       <c r="C92">
         <v>0.02315802704803416</v>
@@ -1406,7 +1406,7 @@
         <v>44011</v>
       </c>
       <c r="B93">
-        <v>0.03010663713174054</v>
+        <v>0.03217847478746445</v>
       </c>
       <c r="C93">
         <v>0.02289672132903939</v>
@@ -1417,7 +1417,7 @@
         <v>44012</v>
       </c>
       <c r="B94">
-        <v>0.02936373335705949</v>
+        <v>0.03141789327558354</v>
       </c>
       <c r="C94">
         <v>0.02243213880033665</v>
@@ -1428,7 +1428,7 @@
         <v>44013</v>
       </c>
       <c r="B95">
-        <v>0.02885213087158912</v>
+        <v>0.03082341774134002</v>
       </c>
       <c r="C95">
         <v>0.02195621833361866</v>
@@ -1439,7 +1439,7 @@
         <v>44014</v>
       </c>
       <c r="B96">
-        <v>0.02825327670436725</v>
+        <v>0.03015830366585575</v>
       </c>
       <c r="C96">
         <v>0.02140964597024392</v>
@@ -1450,7 +1450,7 @@
         <v>44015</v>
       </c>
       <c r="B97">
-        <v>0.02760705145724734</v>
+        <v>0.02945297871936427</v>
       </c>
       <c r="C97">
         <v>0.02087408940017139</v>
@@ -1461,7 +1461,7 @@
         <v>44018</v>
       </c>
       <c r="B98">
-        <v>0.02735396382629871</v>
+        <v>0.02920881959420414</v>
       </c>
       <c r="C98">
         <v>0.0207620026027512</v>
@@ -1472,7 +1472,7 @@
         <v>44019</v>
       </c>
       <c r="B99">
-        <v>0.02704129088183825</v>
+        <v>0.02881530357078537</v>
       </c>
       <c r="C99">
         <v>0.02053901476350315</v>
@@ -1483,7 +1483,7 @@
         <v>44020</v>
       </c>
       <c r="B100">
-        <v>0.02656494083280784</v>
+        <v>0.02829377358864234</v>
       </c>
       <c r="C100">
         <v>0.02035834294532793</v>
@@ -1494,7 +1494,7 @@
         <v>44021</v>
       </c>
       <c r="B101">
-        <v>0.02632597327695359</v>
+        <v>0.02805372238122585</v>
       </c>
       <c r="C101">
         <v>0.01997038475871038</v>
@@ -1505,7 +1505,7 @@
         <v>44022</v>
       </c>
       <c r="B102">
-        <v>0.02580408743195311</v>
+        <v>0.02747563196969195</v>
       </c>
       <c r="C102">
         <v>0.01949601838676423</v>
@@ -1516,7 +1516,7 @@
         <v>44025</v>
       </c>
       <c r="B103">
-        <v>0.02547293805759025</v>
+        <v>0.02711130919739406</v>
       </c>
       <c r="C103">
         <v>0.01937613336841178</v>
@@ -1527,7 +1527,7 @@
         <v>44026</v>
       </c>
       <c r="B104">
-        <v>0.02544378860417749</v>
+        <v>0.02704783566293603</v>
       </c>
       <c r="C104">
         <v>0.01914567960278731</v>
@@ -1538,7 +1538,7 @@
         <v>44027</v>
       </c>
       <c r="B105">
-        <v>0.02496959105466197</v>
+        <v>0.02653488688019549</v>
       </c>
       <c r="C105">
         <v>0.0187770062054403</v>
@@ -1549,7 +1549,7 @@
         <v>44028</v>
       </c>
       <c r="B106">
-        <v>0.02497675579925948</v>
+        <v>0.02655556216514048</v>
       </c>
       <c r="C106">
         <v>0.01865193907061107</v>
@@ -1560,7 +1560,7 @@
         <v>44029</v>
       </c>
       <c r="B107">
-        <v>0.02439333580789959</v>
+        <v>0.02596283294805189</v>
       </c>
       <c r="C107">
         <v>0.01867022305242349</v>
@@ -1571,7 +1571,7 @@
         <v>44032</v>
       </c>
       <c r="B108">
-        <v>0.02382560354453275</v>
+        <v>0.02538946722201665</v>
       </c>
       <c r="C108">
         <v>0.01833849046830223</v>
@@ -1582,7 +1582,7 @@
         <v>44033</v>
       </c>
       <c r="B109">
-        <v>0.0237069031939641</v>
+        <v>0.02522609980884178</v>
       </c>
       <c r="C109">
         <v>0.01792280537562606</v>
@@ -1593,7 +1593,7 @@
         <v>44034</v>
       </c>
       <c r="B110">
-        <v>0.02336296357820897</v>
+        <v>0.02485736375353765</v>
       </c>
       <c r="C110">
         <v>0.01750071654446049</v>
@@ -1604,7 +1604,7 @@
         <v>44035</v>
       </c>
       <c r="B111">
-        <v>0.02316948170413594</v>
+        <v>0.02466321802027989</v>
       </c>
       <c r="C111">
         <v>0.01782463769288837</v>
@@ -1615,7 +1615,7 @@
         <v>44036</v>
       </c>
       <c r="B112">
-        <v>0.02274153140206617</v>
+        <v>0.02413088577204767</v>
       </c>
       <c r="C112">
         <v>0.01738081190654764</v>
@@ -1626,7 +1626,7 @@
         <v>44039</v>
       </c>
       <c r="B113">
-        <v>0.02246028806256021</v>
+        <v>0.02380323585925214</v>
       </c>
       <c r="C113">
         <v>0.0173486501455254</v>
@@ -1637,7 +1637,7 @@
         <v>44040</v>
       </c>
       <c r="B114">
-        <v>0.02246173157243392</v>
+        <v>0.02389856831136998</v>
       </c>
       <c r="C114">
         <v>0.01698782247504588</v>
@@ -1648,7 +1648,7 @@
         <v>44041</v>
       </c>
       <c r="B115">
-        <v>0.0220929612189185</v>
+        <v>0.02351397183518931</v>
       </c>
       <c r="C115">
         <v>0.01672072297196179</v>
@@ -1659,7 +1659,7 @@
         <v>44042</v>
       </c>
       <c r="B116">
-        <v>0.0219273358828981</v>
+        <v>0.02332472660096721</v>
       </c>
       <c r="C116">
         <v>0.01643596186828748</v>
@@ -1670,7 +1670,7 @@
         <v>44043</v>
       </c>
       <c r="B117">
-        <v>0.02211293673992907</v>
+        <v>0.02351305280978415</v>
       </c>
       <c r="C117">
         <v>0.016838443092437</v>
@@ -1681,7 +1681,7 @@
         <v>44046</v>
       </c>
       <c r="B118">
-        <v>0.02179764855533477</v>
+        <v>0.02319061973029302</v>
       </c>
       <c r="C118">
         <v>0.01642719869077577</v>
@@ -1692,7 +1692,7 @@
         <v>44047</v>
       </c>
       <c r="B119">
-        <v>0.02127538768788112</v>
+        <v>0.02262517427422979</v>
       </c>
       <c r="C119">
         <v>0.01648974121730401</v>
@@ -1703,7 +1703,7 @@
         <v>44048</v>
       </c>
       <c r="B120">
-        <v>0.02365351952643331</v>
+        <v>0.0251050336506112</v>
       </c>
       <c r="C120">
         <v>0.01636659320582508</v>
@@ -1714,7 +1714,7 @@
         <v>44049</v>
       </c>
       <c r="B121">
-        <v>0.0233463584311508</v>
+        <v>0.02484876606070452</v>
       </c>
       <c r="C121">
         <v>0.01612233070090515</v>
@@ -1725,7 +1725,7 @@
         <v>44050</v>
       </c>
       <c r="B122">
-        <v>0.02304284190388901</v>
+        <v>0.02457506383335153</v>
       </c>
       <c r="C122">
         <v>0.01608065527152775</v>
@@ -1736,7 +1736,7 @@
         <v>44053</v>
       </c>
       <c r="B123">
-        <v>0.02309821507461161</v>
+        <v>0.02459258542753266</v>
       </c>
       <c r="C123">
         <v>0.01570618249257529</v>
@@ -1747,7 +1747,7 @@
         <v>44054</v>
       </c>
       <c r="B124">
-        <v>0.02273243711377576</v>
+        <v>0.02424587457774459</v>
       </c>
       <c r="C124">
         <v>0.01562760203073764</v>
@@ -1758,7 +1758,7 @@
         <v>44055</v>
       </c>
       <c r="B125">
-        <v>0.02234108337974845</v>
+        <v>0.02382379147889336</v>
       </c>
       <c r="C125">
         <v>0.01523747460324271</v>
@@ -1769,7 +1769,7 @@
         <v>44056</v>
       </c>
       <c r="B126">
-        <v>0.02328173585221718</v>
+        <v>0.02479195049306929</v>
       </c>
       <c r="C126">
         <v>0.01533940485334974</v>
@@ -1780,7 +1780,7 @@
         <v>44057</v>
       </c>
       <c r="B127">
-        <v>0.02278480235173004</v>
+        <v>0.02424804477411377</v>
       </c>
       <c r="C127">
         <v>0.01506459748130586</v>
@@ -1791,7 +1791,7 @@
         <v>44060</v>
       </c>
       <c r="B128">
-        <v>0.02223438353716083</v>
+        <v>0.02367458080067656</v>
       </c>
       <c r="C128">
         <v>0.01521454815404377</v>
@@ -1802,7 +1802,7 @@
         <v>44061</v>
       </c>
       <c r="B129">
-        <v>0.02192258554112553</v>
+        <v>0.02332874428042306</v>
       </c>
       <c r="C129">
         <v>0.01577032312532197</v>
@@ -1813,7 +1813,7 @@
         <v>44062</v>
       </c>
       <c r="B130">
-        <v>0.02142503542050863</v>
+        <v>0.02279580881466857</v>
       </c>
       <c r="C130">
         <v>0.01563168134506598</v>
@@ -1824,7 +1824,7 @@
         <v>44063</v>
       </c>
       <c r="B131">
-        <v>0.02094729086620086</v>
+        <v>0.02229248022805688</v>
       </c>
       <c r="C131">
         <v>0.0152849287572134</v>
@@ -1835,7 +1835,7 @@
         <v>44064</v>
       </c>
       <c r="B132">
-        <v>0.02047428609464758</v>
+        <v>0.0217897249884382</v>
       </c>
       <c r="C132">
         <v>0.01489797876066493</v>
@@ -1846,7 +1846,7 @@
         <v>44067</v>
       </c>
       <c r="B133">
-        <v>0.02015501553442278</v>
+        <v>0.02149976420761373</v>
       </c>
       <c r="C133">
         <v>0.01459839162670249</v>
@@ -1857,7 +1857,7 @@
         <v>44068</v>
       </c>
       <c r="B134">
-        <v>0.0197115452199846</v>
+        <v>0.02102094699496305</v>
       </c>
       <c r="C134">
         <v>0.0142421290898614</v>
@@ -1868,7 +1868,7 @@
         <v>44069</v>
       </c>
       <c r="B135">
-        <v>0.01881977418700417</v>
+        <v>0.02059405931862156</v>
       </c>
       <c r="C135">
         <v>0.01429374984366692</v>
@@ -1879,7 +1879,7 @@
         <v>44070</v>
       </c>
       <c r="B136">
-        <v>0.01825470923832667</v>
+        <v>0.02010523127784546</v>
       </c>
       <c r="C136">
         <v>0.01393187733684243</v>
@@ -1890,7 +1890,7 @@
         <v>44071</v>
       </c>
       <c r="B137">
-        <v>0.01800778769429625</v>
+        <v>0.01991056291221425</v>
       </c>
       <c r="C137">
         <v>0.01395921981814569</v>
@@ -1901,7 +1901,7 @@
         <v>44074</v>
       </c>
       <c r="B138">
-        <v>0.01826295658744211</v>
+        <v>0.02019261013570282</v>
       </c>
       <c r="C138">
         <v>0.01494878988333008</v>
@@ -1912,7 +1912,7 @@
         <v>44075</v>
       </c>
       <c r="B139">
-        <v>0.0192565555189162</v>
+        <v>0.02128949317212599</v>
       </c>
       <c r="C139">
         <v>0.01582356643070262</v>
@@ -1923,7 +1923,7 @@
         <v>44076</v>
       </c>
       <c r="B140">
-        <v>0.01887565548551846</v>
+        <v>0.02089651477938656</v>
       </c>
       <c r="C140">
         <v>0.01544063643168531</v>
@@ -1934,7 +1934,7 @@
         <v>44077</v>
       </c>
       <c r="B141">
-        <v>0.01857602302166008</v>
+        <v>0.02055438178084237</v>
       </c>
       <c r="C141">
         <v>0.01529238395248634</v>
@@ -1945,7 +1945,7 @@
         <v>44078</v>
       </c>
       <c r="B142">
-        <v>0.01811352960362806</v>
+        <v>0.0200453487153392</v>
       </c>
       <c r="C142">
         <v>0.01494617101437484</v>
@@ -1956,7 +1956,7 @@
         <v>44082</v>
       </c>
       <c r="B143">
-        <v>0.01827488712025289</v>
+        <v>0.0202389681529446</v>
       </c>
       <c r="C143">
         <v>0.01480764330229952</v>
@@ -1967,7 +1967,7 @@
         <v>44083</v>
       </c>
       <c r="B144">
-        <v>0.01815741367174272</v>
+        <v>0.02008246489741232</v>
       </c>
       <c r="C144">
         <v>0.01469200955173569</v>
@@ -1978,7 +1978,7 @@
         <v>44084</v>
       </c>
       <c r="B145">
-        <v>0.01835816819944463</v>
+        <v>0.02036898073852141</v>
       </c>
       <c r="C145">
         <v>0.01531491299246796</v>
@@ -1989,7 +1989,7 @@
         <v>44085</v>
       </c>
       <c r="B146">
-        <v>0.01808631682384722</v>
+        <v>0.02005632989664974</v>
       </c>
       <c r="C146">
         <v>0.01495131075971683</v>
@@ -2000,7 +2000,7 @@
         <v>44088</v>
       </c>
       <c r="B147">
-        <v>0.01779177592078674</v>
+        <v>0.01979652225300849</v>
       </c>
       <c r="C147">
         <v>0.01523168183151306</v>
@@ -2011,7 +2011,7 @@
         <v>44089</v>
       </c>
       <c r="B148">
-        <v>0.01760218818731301</v>
+        <v>0.01962049532654314</v>
       </c>
       <c r="C148">
         <v>0.01484614602861528</v>
@@ -2022,7 +2022,7 @@
         <v>44090</v>
       </c>
       <c r="B149">
-        <v>0.01722010736536175</v>
+        <v>0.01918105842598971</v>
       </c>
       <c r="C149">
         <v>0.01453258435220602</v>
@@ -2033,7 +2033,7 @@
         <v>44091</v>
       </c>
       <c r="B150">
-        <v>0.01709924773984246</v>
+        <v>0.01902292777282399</v>
       </c>
       <c r="C150">
         <v>0.01419979980768377</v>
@@ -2044,7 +2044,7 @@
         <v>44092</v>
       </c>
       <c r="B151">
-        <v>0.01713505822502565</v>
+        <v>0.01905858875436799</v>
       </c>
       <c r="C151">
         <v>0.01439130439149726</v>
@@ -2055,7 +2055,7 @@
         <v>44095</v>
       </c>
       <c r="B152">
-        <v>0.01751219975385985</v>
+        <v>0.01949180911838925</v>
       </c>
       <c r="C152">
         <v>0.01427951457575623</v>
@@ -2066,7 +2066,7 @@
         <v>44096</v>
       </c>
       <c r="B153">
-        <v>0.01709451252536733</v>
+        <v>0.01902199444953679</v>
       </c>
       <c r="C153">
         <v>0.01395668011570335</v>
@@ -2077,7 +2077,7 @@
         <v>44097</v>
       </c>
       <c r="B154">
-        <v>0.0172558113510414</v>
+        <v>0.01919554275082813</v>
       </c>
       <c r="C154">
         <v>0.0139776416044824</v>
@@ -2088,7 +2088,7 @@
         <v>44098</v>
       </c>
       <c r="B155">
-        <v>0.01698868941624044</v>
+        <v>0.01889648549305296</v>
       </c>
       <c r="C155">
         <v>0.01403095474614657</v>
@@ -2099,7 +2099,7 @@
         <v>44099</v>
       </c>
       <c r="B156">
-        <v>0.01663310081969149</v>
+        <v>0.01850309512886171</v>
       </c>
       <c r="C156">
         <v>0.01367836693293967</v>
@@ -2110,7 +2110,7 @@
         <v>44102</v>
       </c>
       <c r="B157">
-        <v>0.01683356955146276</v>
+        <v>0.01872441108319407</v>
       </c>
       <c r="C157">
         <v>0.01424561142863418</v>
@@ -2121,7 +2121,7 @@
         <v>44103</v>
       </c>
       <c r="B158">
-        <v>0.01662526039902617</v>
+        <v>0.01848319461393083</v>
       </c>
       <c r="C158">
         <v>0.0140249616741015</v>
@@ -2132,7 +2132,7 @@
         <v>44104</v>
       </c>
       <c r="B159">
-        <v>0.01642509107535707</v>
+        <v>0.01828739500814404</v>
       </c>
       <c r="C159">
         <v>0.01399645982766371</v>
@@ -2143,7 +2143,7 @@
         <v>44105</v>
       </c>
       <c r="B160">
-        <v>0.01625004870036353</v>
+        <v>0.01808435933049446</v>
       </c>
       <c r="C160">
         <v>0.01386833442466498</v>
@@ -2154,7 +2154,7 @@
         <v>44106</v>
       </c>
       <c r="B161">
-        <v>0.01687030438049093</v>
+        <v>0.01880073906693519</v>
       </c>
       <c r="C161">
         <v>0.01384695019144099</v>
@@ -2165,7 +2165,7 @@
         <v>44109</v>
       </c>
       <c r="B162">
-        <v>0.01859767913046561</v>
+        <v>0.02067729473868826</v>
       </c>
       <c r="C162">
         <v>0.014486914569428</v>
@@ -2176,7 +2176,7 @@
         <v>44110</v>
       </c>
       <c r="B163">
-        <v>0.01812508255803404</v>
+        <v>0.02015348010266833</v>
       </c>
       <c r="C163">
         <v>0.01414443731455185</v>
@@ -2187,7 +2187,7 @@
         <v>44111</v>
       </c>
       <c r="B164">
-        <v>0.01769738444870857</v>
+        <v>0.01967293597130019</v>
       </c>
       <c r="C164">
         <v>0.01378656573124883</v>
@@ -2198,7 +2198,7 @@
         <v>44112</v>
       </c>
       <c r="B165">
-        <v>0.01845723728161795</v>
+        <v>0.02051299210151573</v>
       </c>
       <c r="C165">
         <v>0.01458868379816073</v>
@@ -2209,7 +2209,7 @@
         <v>44113</v>
       </c>
       <c r="B166">
-        <v>0.01857008493730485</v>
+        <v>0.02065476011150861</v>
       </c>
       <c r="C166">
         <v>0.01425256635377702</v>
@@ -2220,7 +2220,7 @@
         <v>44117</v>
       </c>
       <c r="B167">
-        <v>0.01861004046716387</v>
+        <v>0.02069667697643008</v>
       </c>
       <c r="C167">
         <v>0.01408386776303857</v>
@@ -2231,7 +2231,7 @@
         <v>44118</v>
       </c>
       <c r="B168">
-        <v>0.01826726599303843</v>
+        <v>0.02034862773978729</v>
       </c>
       <c r="C168">
         <v>0.0138402763564142</v>
@@ -2242,7 +2242,7 @@
         <v>44119</v>
       </c>
       <c r="B169">
-        <v>0.01784942951385878</v>
+        <v>0.01988781150845854</v>
       </c>
       <c r="C169">
         <v>0.01351174884725847</v>
@@ -2253,7 +2253,7 @@
         <v>44120</v>
       </c>
       <c r="B170">
-        <v>0.01762874991131672</v>
+        <v>0.0196607694987727</v>
       </c>
       <c r="C170">
         <v>0.01328683836730531</v>
@@ -2264,7 +2264,7 @@
         <v>44123</v>
       </c>
       <c r="B171">
-        <v>0.01748398156136081</v>
+        <v>0.0194825650773082</v>
       </c>
       <c r="C171">
         <v>0.01297180738421976</v>
@@ -2275,7 +2275,7 @@
         <v>44124</v>
       </c>
       <c r="B172">
-        <v>0.01815388873636868</v>
+        <v>0.02021912094686595</v>
       </c>
       <c r="C172">
         <v>0.01327726815675187</v>
@@ -2286,7 +2286,7 @@
         <v>44125</v>
       </c>
       <c r="B173">
-        <v>0.01774703822160533</v>
+        <v>0.01975943884122672</v>
       </c>
       <c r="C173">
         <v>0.0129433325605964</v>
@@ -2297,7 +2297,7 @@
         <v>44126</v>
       </c>
       <c r="B174">
-        <v>0.01835367886338722</v>
+        <v>0.02046735059832953</v>
       </c>
       <c r="C174">
         <v>0.01289825801583431</v>
@@ -2308,7 +2308,7 @@
         <v>44127</v>
       </c>
       <c r="B175">
-        <v>0.01809292290505185</v>
+        <v>0.02017268723373093</v>
       </c>
       <c r="C175">
         <v>0.0127000612008801</v>
@@ -2319,7 +2319,7 @@
         <v>44130</v>
       </c>
       <c r="B176">
-        <v>0.01785892729314217</v>
+        <v>0.01991895239478882</v>
       </c>
       <c r="C176">
         <v>0.01240583370928261</v>
@@ -2330,7 +2330,7 @@
         <v>44131</v>
       </c>
       <c r="B177">
-        <v>0.01783691154227955</v>
+        <v>0.01987994875908905</v>
       </c>
       <c r="C177">
         <v>0.01254031097933074</v>
@@ -2341,7 +2341,7 @@
         <v>44132</v>
       </c>
       <c r="B178">
-        <v>0.01980356097427791</v>
+        <v>0.02209370966590053</v>
       </c>
       <c r="C178">
         <v>0.01552113379567822</v>
@@ -2352,7 +2352,7 @@
         <v>44133</v>
       </c>
       <c r="B179">
-        <v>0.02013420513831791</v>
+        <v>0.02242728003904718</v>
       </c>
       <c r="C179">
         <v>0.01545069275725872</v>
@@ -2363,7 +2363,7 @@
         <v>44134</v>
       </c>
       <c r="B180">
-        <v>0.01979173169607982</v>
+        <v>0.02204708336320893</v>
       </c>
       <c r="C180">
         <v>0.01613348781357945</v>
@@ -2374,7 +2374,7 @@
         <v>44138</v>
       </c>
       <c r="B181">
-        <v>0.02038689590973099</v>
+        <v>0.02268231818339824</v>
       </c>
       <c r="C181">
         <v>0.01629666918307288</v>
@@ -2385,7 +2385,7 @@
         <v>44139</v>
       </c>
       <c r="B182">
-        <v>0.01998967640743235</v>
+        <v>0.02225143537952117</v>
       </c>
       <c r="C182">
         <v>0.01675040185879883</v>
@@ -2396,7 +2396,7 @@
         <v>44140</v>
       </c>
       <c r="B183">
-        <v>0.0196983420523728</v>
+        <v>0.02193575297604333</v>
       </c>
       <c r="C183">
         <v>0.01758852140962025</v>
@@ -2407,7 +2407,7 @@
         <v>44141</v>
       </c>
       <c r="B184">
-        <v>0.01920800267045045</v>
+        <v>0.02139880031136578</v>
       </c>
       <c r="C184">
         <v>0.01714477297941915</v>
@@ -2418,7 +2418,7 @@
         <v>44144</v>
       </c>
       <c r="B185">
-        <v>0.02377211272279188</v>
+        <v>0.02642300024268077</v>
       </c>
       <c r="C185">
         <v>0.01787801859711558</v>
@@ -2429,7 +2429,7 @@
         <v>44145</v>
       </c>
       <c r="B186">
-        <v>0.02557761260725965</v>
+        <v>0.02836856546271735</v>
       </c>
       <c r="C186">
         <v>0.01758995493807026</v>
@@ -2440,7 +2440,7 @@
         <v>44146</v>
       </c>
       <c r="B187">
-        <v>0.02511696519209767</v>
+        <v>0.02784953821621312</v>
       </c>
       <c r="C187">
         <v>0.0173138856324691</v>
@@ -2451,7 +2451,7 @@
         <v>44147</v>
       </c>
       <c r="B188">
-        <v>0.02547097785242291</v>
+        <v>0.02829078522530795</v>
       </c>
       <c r="C188">
         <v>0.01776916111884218</v>
@@ -2462,7 +2462,7 @@
         <v>44148</v>
       </c>
       <c r="B189">
-        <v>0.02535998010830808</v>
+        <v>0.0281399315189562</v>
       </c>
       <c r="C189">
         <v>0.01792311356179039</v>
@@ -2473,7 +2473,7 @@
         <v>44151</v>
       </c>
       <c r="B190">
-        <v>0.02429734961685802</v>
+        <v>0.02731145342789881</v>
       </c>
       <c r="C190">
         <v>0.01780038454662054</v>
@@ -2484,7 +2484,7 @@
         <v>44152</v>
       </c>
       <c r="B191">
-        <v>0.0235287804217989</v>
+        <v>0.02656337962842685</v>
       </c>
       <c r="C191">
         <v>0.01737367428733777</v>
@@ -2495,7 +2495,7 @@
         <v>44153</v>
       </c>
       <c r="B192">
-        <v>0.02296577199850312</v>
+        <v>0.02605324359656579</v>
       </c>
       <c r="C192">
         <v>0.01708713735332522</v>
@@ -2506,7 +2506,7 @@
         <v>44154</v>
       </c>
       <c r="B193">
-        <v>0.02258826944075557</v>
+        <v>0.02561044532328308</v>
       </c>
       <c r="C193">
         <v>0.01666454045164718</v>
@@ -2517,7 +2517,7 @@
         <v>44158</v>
       </c>
       <c r="B194">
-        <v>0.0227387420388511</v>
+        <v>0.02596723227834788</v>
       </c>
       <c r="C194">
         <v>0.01628233768446739</v>
@@ -2528,7 +2528,7 @@
         <v>44159</v>
       </c>
       <c r="B195">
-        <v>0.02243779322607425</v>
+        <v>0.02575553691988501</v>
       </c>
       <c r="C195">
         <v>0.01640498150302605</v>
@@ -2539,7 +2539,7 @@
         <v>44160</v>
       </c>
       <c r="B196">
-        <v>0.02212766805645679</v>
+        <v>0.02533050517932661</v>
       </c>
       <c r="C196">
         <v>0.01599080421116513</v>
@@ -2550,7 +2550,7 @@
         <v>44161</v>
       </c>
       <c r="B197">
-        <v>0.0213027064114496</v>
+        <v>0.02461471220317872</v>
       </c>
       <c r="C197">
         <v>0.01560110367313191</v>
@@ -2561,7 +2561,7 @@
         <v>44162</v>
       </c>
       <c r="B198">
-        <v>0.02088901271444771</v>
+        <v>0.02415649798776218</v>
       </c>
       <c r="C198">
         <v>0.01520684394520182</v>
@@ -2572,7 +2572,7 @@
         <v>44165</v>
       </c>
       <c r="B199">
-        <v>0.0206299300494403</v>
+        <v>0.02391550653329983</v>
       </c>
       <c r="C199">
         <v>0.015400755360385</v>
@@ -2583,7 +2583,7 @@
         <v>44166</v>
       </c>
       <c r="B200">
-        <v>0.02065742409157053</v>
+        <v>0.02393035578877139</v>
       </c>
       <c r="C200">
         <v>0.01559282659983271</v>
@@ -2594,7 +2594,7 @@
         <v>44167</v>
       </c>
       <c r="B201">
-        <v>0.02028631842622741</v>
+        <v>0.02345968927354138</v>
       </c>
       <c r="C201">
         <v>0.01519834638573331</v>
@@ -2605,7 +2605,7 @@
         <v>44168</v>
       </c>
       <c r="B202">
-        <v>0.02006606406134094</v>
+        <v>0.02317527069132151</v>
       </c>
       <c r="C202">
         <v>0.014870802087532</v>
@@ -2616,7 +2616,7 @@
         <v>44169</v>
       </c>
       <c r="B203">
-        <v>0.02000561467249597</v>
+        <v>0.02307446549404369</v>
       </c>
       <c r="C203">
         <v>0.01450520610394766</v>
@@ -2627,7 +2627,7 @@
         <v>44172</v>
       </c>
       <c r="B204">
-        <v>0.01972162762965284</v>
+        <v>0.02278241308135255</v>
       </c>
       <c r="C204">
         <v>0.01417626566926466</v>
@@ -2638,7 +2638,7 @@
         <v>44173</v>
       </c>
       <c r="B205">
-        <v>0.01989260858828921</v>
+        <v>0.02305316437511554</v>
       </c>
       <c r="C205">
         <v>0.01385231532936489</v>
@@ -2649,7 +2649,7 @@
         <v>44174</v>
       </c>
       <c r="B206">
-        <v>0.01955181189521553</v>
+        <v>0.02262981723426033</v>
       </c>
       <c r="C206">
         <v>0.01372504028975296</v>
@@ -2660,7 +2660,7 @@
         <v>44175</v>
       </c>
       <c r="B207">
-        <v>0.01961636370302807</v>
+        <v>0.0226756335000085</v>
       </c>
       <c r="C207">
         <v>0.01386321300674856</v>
@@ -2671,7 +2671,7 @@
         <v>44176</v>
       </c>
       <c r="B208">
-        <v>0.01925906867516613</v>
+        <v>0.02226689382303591</v>
       </c>
       <c r="C208">
         <v>0.01351475541828988</v>
@@ -2682,7 +2682,7 @@
         <v>44179</v>
       </c>
       <c r="B209">
-        <v>0.01891683043940653</v>
+        <v>0.02185875611982463</v>
       </c>
       <c r="C209">
         <v>0.01326172773436942</v>
@@ -2693,7 +2693,7 @@
         <v>44180</v>
       </c>
       <c r="B210">
-        <v>0.01847703491916266</v>
+        <v>0.02134546859102233</v>
       </c>
       <c r="C210">
         <v>0.01300245839217293</v>
@@ -2704,7 +2704,7 @@
         <v>44181</v>
       </c>
       <c r="B211">
-        <v>0.01810360663854856</v>
+        <v>0.0209158743579666</v>
       </c>
       <c r="C211">
         <v>0.01291423056850661</v>
@@ -2715,7 +2715,7 @@
         <v>44182</v>
       </c>
       <c r="B212">
-        <v>0.01771498735949073</v>
+        <v>0.02045813405744524</v>
       </c>
       <c r="C212">
         <v>0.01260185228590875</v>
@@ -2726,7 +2726,7 @@
         <v>44183</v>
       </c>
       <c r="B213">
-        <v>0.01733277305312252</v>
+        <v>0.02002861434385053</v>
       </c>
       <c r="C213">
         <v>0.01242095301662802</v>
@@ -2737,7 +2737,7 @@
         <v>44186</v>
       </c>
       <c r="B214">
-        <v>0.01771221952684226</v>
+        <v>0.02057067343803598</v>
       </c>
       <c r="C214">
         <v>0.01274190209652336</v>
@@ -2748,7 +2748,7 @@
         <v>44187</v>
       </c>
       <c r="B215">
-        <v>0.01738976739577689</v>
+        <v>0.02018202208365526</v>
       </c>
       <c r="C215">
         <v>0.01241937174695864</v>
@@ -2759,7 +2759,7 @@
         <v>44188</v>
       </c>
       <c r="B216">
-        <v>0.01704659251315512</v>
+        <v>0.01979468394711844</v>
       </c>
       <c r="C216">
         <v>0.01229225502241317</v>
@@ -2770,7 +2770,7 @@
         <v>44193</v>
       </c>
       <c r="B217">
-        <v>0.01665999532905461</v>
+        <v>0.01933553827358469</v>
       </c>
       <c r="C217">
         <v>0.01206479457516466</v>
@@ -2781,7 +2781,7 @@
         <v>44194</v>
       </c>
       <c r="B218">
-        <v>0.01628578031728465</v>
+        <v>0.01890249498903001</v>
       </c>
       <c r="C218">
         <v>0.01175953752127514</v>
@@ -2792,7 +2792,7 @@
         <v>44195</v>
       </c>
       <c r="B219">
-        <v>0.01606006330940199</v>
+        <v>0.01862154599467938</v>
       </c>
       <c r="C219">
         <v>0.01151965300900876</v>
@@ -2803,7 +2803,7 @@
         <v>44200</v>
       </c>
       <c r="B220">
-        <v>0.01615387232686241</v>
+        <v>0.01872772123016952</v>
       </c>
       <c r="C220">
         <v>0.01143343707161859</v>
@@ -2814,7 +2814,7 @@
         <v>44201</v>
       </c>
       <c r="B221">
-        <v>0.01628707337886587</v>
+        <v>0.01884886614686952</v>
       </c>
       <c r="C221">
         <v>0.01115700433004003</v>
@@ -2825,7 +2825,7 @@
         <v>44202</v>
       </c>
       <c r="B222">
-        <v>0.01609941779252898</v>
+        <v>0.01864198345097201</v>
       </c>
       <c r="C222">
         <v>0.01088335224315583</v>
@@ -2836,7 +2836,7 @@
         <v>44203</v>
       </c>
       <c r="B223">
-        <v>0.01645723337010974</v>
+        <v>0.01905070122950738</v>
       </c>
       <c r="C223">
         <v>0.01104212183035747</v>
@@ -2847,7 +2847,7 @@
         <v>44204</v>
       </c>
       <c r="B224">
-        <v>0.01610791174520405</v>
+        <v>0.0186512585496466</v>
       </c>
       <c r="C224">
         <v>0.01171453826379001</v>
@@ -2858,7 +2858,7 @@
         <v>44207</v>
       </c>
       <c r="B225">
-        <v>0.01605349394888447</v>
+        <v>0.01857825749716082</v>
       </c>
       <c r="C225">
         <v>0.01250700298117306</v>
@@ -2869,7 +2869,7 @@
         <v>44208</v>
       </c>
       <c r="B226">
-        <v>0.01589410514683033</v>
+        <v>0.01840275820300385</v>
       </c>
       <c r="C226">
         <v>0.01225382637530642</v>
@@ -2880,7 +2880,7 @@
         <v>44209</v>
       </c>
       <c r="B227">
-        <v>0.01700333470691873</v>
+        <v>0.01972865814546962</v>
       </c>
       <c r="C227">
         <v>0.01272437351596991</v>
@@ -2891,7 +2891,7 @@
         <v>44210</v>
       </c>
       <c r="B228">
-        <v>0.01678016404022576</v>
+        <v>0.01944508193738623</v>
       </c>
       <c r="C228">
         <v>0.0125405806526634</v>
@@ -2902,7 +2902,7 @@
         <v>44211</v>
       </c>
       <c r="B229">
-        <v>0.01787024172626309</v>
+        <v>0.02072279350409712</v>
       </c>
       <c r="C229">
         <v>0.01366765219724051</v>
@@ -2913,7 +2913,7 @@
         <v>44214</v>
       </c>
       <c r="B230">
-        <v>0.0174860579620171</v>
+        <v>0.02027058245530413</v>
       </c>
       <c r="C230">
         <v>0.0133484664599652</v>
@@ -2924,7 +2924,7 @@
         <v>44215</v>
       </c>
       <c r="B231">
-        <v>0.01734308118763874</v>
+        <v>0.02007897904061623</v>
       </c>
       <c r="C231">
         <v>0.01310308209529184</v>
@@ -2935,7 +2935,7 @@
         <v>44216</v>
       </c>
       <c r="B232">
-        <v>0.0171432635303833</v>
+        <v>0.01986288619116252</v>
       </c>
       <c r="C232">
         <v>0.01295973904945046</v>
@@ -2946,7 +2946,7 @@
         <v>44217</v>
       </c>
       <c r="B233">
-        <v>0.01700855349415156</v>
+        <v>0.01972133641441228</v>
       </c>
       <c r="C233">
         <v>0.01290808274977002</v>
@@ -2957,7 +2957,7 @@
         <v>44218</v>
       </c>
       <c r="B234">
-        <v>0.0168214375570956</v>
+        <v>0.01953147891318641</v>
       </c>
       <c r="C234">
         <v>0.01283915300391391</v>
@@ -2968,7 +2968,7 @@
         <v>44222</v>
       </c>
       <c r="B235">
-        <v>0.01664485899292293</v>
+        <v>0.01930967405951095</v>
       </c>
       <c r="C235">
         <v>0.01259234924510601</v>
@@ -2979,7 +2979,7 @@
         <v>44223</v>
       </c>
       <c r="B236">
-        <v>0.01655440405223305</v>
+        <v>0.01919747336745939</v>
       </c>
       <c r="C236">
         <v>0.01232295321391926</v>
@@ -2990,7 +2990,7 @@
         <v>44224</v>
       </c>
       <c r="B237">
-        <v>0.01661469210505449</v>
+        <v>0.01928156502770408</v>
       </c>
       <c r="C237">
         <v>0.01361206313745144</v>
@@ -3001,7 +3001,7 @@
         <v>44225</v>
       </c>
       <c r="B238">
-        <v>0.01722781047650801</v>
+        <v>0.02000091217063498</v>
       </c>
       <c r="C238">
         <v>0.01473129974094322</v>
@@ -3012,7 +3012,7 @@
         <v>44228</v>
       </c>
       <c r="B239">
-        <v>0.01749850220595755</v>
+        <v>0.02028763320426845</v>
       </c>
       <c r="C239">
         <v>0.0145883356698968</v>
@@ -3023,7 +3023,7 @@
         <v>44229</v>
       </c>
       <c r="B240">
-        <v>0.01807777151387323</v>
+        <v>0.02093861698793149</v>
       </c>
       <c r="C240">
         <v>0.01430025602646649</v>
@@ -3034,7 +3034,7 @@
         <v>44230</v>
       </c>
       <c r="B241">
-        <v>0.01780079421468587</v>
+        <v>0.02062548496781496</v>
       </c>
       <c r="C241">
         <v>0.01417313260767493</v>
@@ -3045,7 +3045,7 @@
         <v>44231</v>
       </c>
       <c r="B242">
-        <v>0.01740889588777131</v>
+        <v>0.02019129964233076</v>
       </c>
       <c r="C242">
         <v>0.0138608880623055</v>
@@ -3056,7 +3056,7 @@
         <v>44232</v>
       </c>
       <c r="B243">
-        <v>0.01709223844704782</v>
+        <v>0.01984849577743615</v>
       </c>
       <c r="C243">
         <v>0.01354521789813944</v>
@@ -3067,7 +3067,7 @@
         <v>44235</v>
       </c>
       <c r="B244">
-        <v>0.01704552701687858</v>
+        <v>0.01984451417490298</v>
       </c>
       <c r="C244">
         <v>0.01324207530088741</v>
@@ -3078,7 +3078,7 @@
         <v>44236</v>
       </c>
       <c r="B245">
-        <v>0.01676639407523268</v>
+        <v>0.01955287611662683</v>
       </c>
       <c r="C245">
         <v>0.01291264288178941</v>
@@ -3089,7 +3089,7 @@
         <v>44237</v>
       </c>
       <c r="B246">
-        <v>0.01649158768482623</v>
+        <v>0.01923428825213367</v>
       </c>
       <c r="C246">
         <v>0.01275021707069045</v>
@@ -3100,7 +3100,7 @@
         <v>44238</v>
       </c>
       <c r="B247">
-        <v>0.01624409132933548</v>
+        <v>0.01895458752904442</v>
       </c>
       <c r="C247">
         <v>0.01250239215891648</v>
@@ -3111,7 +3111,7 @@
         <v>44239</v>
       </c>
       <c r="B248">
-        <v>0.01592208546278116</v>
+        <v>0.01858483037201529</v>
       </c>
       <c r="C248">
         <v>0.01219222068325578</v>
@@ -3122,7 +3122,7 @@
         <v>44245</v>
       </c>
       <c r="B249">
-        <v>0.01618328492053868</v>
+        <v>0.01887155064764892</v>
       </c>
       <c r="C249">
         <v>0.01188404971484599</v>
@@ -3133,7 +3133,7 @@
         <v>44246</v>
       </c>
       <c r="B250">
-        <v>0.01763524196762472</v>
+        <v>0.02059995326737996</v>
       </c>
       <c r="C250">
         <v>0.01161577302937092</v>
@@ -3144,7 +3144,7 @@
         <v>44249</v>
       </c>
       <c r="B251">
-        <v>0.02738325701565444</v>
+        <v>0.03259431450061362</v>
       </c>
       <c r="C251">
         <v>0.01618287123338495</v>
@@ -3155,7 +3155,7 @@
         <v>44250</v>
       </c>
       <c r="B252">
-        <v>0.02911895266402554</v>
+        <v>0.0345643147039472</v>
       </c>
       <c r="C252">
         <v>0.01666042661275628</v>
@@ -3166,7 +3166,7 @@
         <v>44251</v>
       </c>
       <c r="B253">
-        <v>0.02917735820883437</v>
+        <v>0.03453464144837076</v>
       </c>
       <c r="C253">
         <v>0.01627147085827648</v>
@@ -3177,7 +3177,7 @@
         <v>44252</v>
       </c>
       <c r="B254">
-        <v>0.02884186386452474</v>
+        <v>0.03414089702958096</v>
       </c>
       <c r="C254">
         <v>0.01709309204104374</v>
@@ -3188,7 +3188,7 @@
         <v>44253</v>
       </c>
       <c r="B255">
-        <v>0.02866118256266666</v>
+        <v>0.03389668781076548</v>
       </c>
       <c r="C255">
         <v>0.01710762532270184</v>
@@ -3199,7 +3199,7 @@
         <v>44256</v>
       </c>
       <c r="B256">
-        <v>0.02811502460881442</v>
+        <v>0.03327404561232482</v>
       </c>
       <c r="C256">
         <v>0.01672171895092601</v>
@@ -3210,7 +3210,7 @@
         <v>44257</v>
       </c>
       <c r="B257">
-        <v>0.0275540446363971</v>
+        <v>0.03260069423813235</v>
       </c>
       <c r="C257">
         <v>0.01656627127585181</v>
@@ -3221,7 +3221,7 @@
         <v>44258</v>
       </c>
       <c r="B258">
-        <v>0.02680825628168548</v>
+        <v>0.03176487021538265</v>
       </c>
       <c r="C258">
         <v>0.01614866104568067</v>
@@ -3232,7 +3232,7 @@
         <v>44259</v>
       </c>
       <c r="B259">
-        <v>0.02716235122455522</v>
+        <v>0.03218205818644546</v>
       </c>
       <c r="C259">
         <v>0.01610203170403202</v>
@@ -3243,7 +3243,7 @@
         <v>44260</v>
       </c>
       <c r="B260">
-        <v>0.0269165949005064</v>
+        <v>0.03193242597734267</v>
       </c>
       <c r="C260">
         <v>0.0165019103624093</v>
@@ -3254,7 +3254,7 @@
         <v>44263</v>
       </c>
       <c r="B261">
-        <v>0.02652734874067668</v>
+        <v>0.03151860870228651</v>
       </c>
       <c r="C261">
         <v>0.01834463372576453</v>
@@ -3265,7 +3265,7 @@
         <v>44264</v>
       </c>
       <c r="B262">
-        <v>0.02613969512275857</v>
+        <v>0.03124092830396932</v>
       </c>
       <c r="C262">
         <v>0.01798001226472664</v>
@@ -3276,7 +3276,7 @@
         <v>44265</v>
       </c>
       <c r="B263">
-        <v>0.02625376267850221</v>
+        <v>0.03133918336962023</v>
       </c>
       <c r="C263">
         <v>0.0178138545156474</v>
@@ -3287,7 +3287,7 @@
         <v>44266</v>
       </c>
       <c r="B264">
-        <v>0.0262474068286252</v>
+        <v>0.0313131405530221</v>
       </c>
       <c r="C264">
         <v>0.01792442740464835</v>
@@ -3298,7 +3298,7 @@
         <v>44267</v>
       </c>
       <c r="B265">
-        <v>0.02577213456145771</v>
+        <v>0.03073624498539885</v>
       </c>
       <c r="C265">
         <v>0.01754044627436281</v>
@@ -3309,7 +3309,7 @@
         <v>44270</v>
       </c>
       <c r="B266">
-        <v>0.0254114992520784</v>
+        <v>0.03029450430328015</v>
       </c>
       <c r="C266">
         <v>0.01715327721430302</v>
@@ -3320,7 +3320,7 @@
         <v>44271</v>
       </c>
       <c r="B267">
-        <v>0.0247844645274492</v>
+        <v>0.02959598981650708</v>
       </c>
       <c r="C267">
         <v>0.01679276708491401</v>
@@ -3331,7 +3331,7 @@
         <v>44272</v>
       </c>
       <c r="B268">
-        <v>0.0245544330133944</v>
+        <v>0.02935898168012673</v>
       </c>
       <c r="C268">
         <v>0.01707772108369376</v>
@@ -3342,7 +3342,7 @@
         <v>44273</v>
       </c>
       <c r="B269">
-        <v>0.02346707666292831</v>
+        <v>0.0284997907054078</v>
       </c>
       <c r="C269">
         <v>0.01698545958674685</v>
@@ -3353,7 +3353,7 @@
         <v>44274</v>
       </c>
       <c r="B270">
-        <v>0.02328923907297723</v>
+        <v>0.02831247085504314</v>
       </c>
       <c r="C270">
         <v>0.01676335802189397</v>
@@ -3364,7 +3364,7 @@
         <v>44277</v>
       </c>
       <c r="B271">
-        <v>0.02248555472117487</v>
+        <v>0.02755066517640822</v>
       </c>
       <c r="C271">
         <v>0.01652294841300216</v>
@@ -3375,7 +3375,7 @@
         <v>44278</v>
       </c>
       <c r="B272">
-        <v>0.02130678005188088</v>
+        <v>0.02679052656273765</v>
       </c>
       <c r="C272">
         <v>0.0164336067652741</v>
@@ -3386,7 +3386,7 @@
         <v>44279</v>
       </c>
       <c r="B273">
-        <v>0.01997658848109124</v>
+        <v>0.02576340430174478</v>
       </c>
       <c r="C273">
         <v>0.01616072231296432</v>
@@ -3397,7 +3397,7 @@
         <v>44280</v>
       </c>
       <c r="B274">
-        <v>0.0186390491588539</v>
+        <v>0.02475478861963666</v>
       </c>
       <c r="C274">
         <v>0.01614280259055818</v>
@@ -3408,7 +3408,7 @@
         <v>44281</v>
       </c>
       <c r="B275">
-        <v>0.01840387859150727</v>
+        <v>0.02439890502430123</v>
       </c>
       <c r="C275">
         <v>0.01586937326412589</v>
@@ -3419,7 +3419,7 @@
         <v>44284</v>
       </c>
       <c r="B276">
-        <v>0.01740814951342857</v>
+        <v>0.02356377406661699</v>
       </c>
       <c r="C276">
         <v>0.0155145065798891</v>
@@ -3430,7 +3430,7 @@
         <v>44285</v>
       </c>
       <c r="B277">
-        <v>0.01727749640991654</v>
+        <v>0.02317567284371888</v>
       </c>
       <c r="C277">
         <v>0.01534752602325721</v>
@@ -3441,7 +3441,7 @@
         <v>44286</v>
       </c>
       <c r="B278">
-        <v>0.01692293384032914</v>
+        <v>0.02273391575266237</v>
       </c>
       <c r="C278">
         <v>0.01497081263507121</v>
@@ -3452,7 +3452,7 @@
         <v>44287</v>
       </c>
       <c r="B279">
-        <v>0.01666465971519126</v>
+        <v>0.02240914350334505</v>
       </c>
       <c r="C279">
         <v>0.0148503892356783</v>
@@ -3463,7 +3463,7 @@
         <v>44292</v>
       </c>
       <c r="B280">
-        <v>0.01571281132659843</v>
+        <v>0.02154433436386832</v>
       </c>
       <c r="C280">
         <v>0.01469665623144918</v>
@@ -3474,7 +3474,7 @@
         <v>44293</v>
       </c>
       <c r="B281">
-        <v>0.01507261010456809</v>
+        <v>0.02088894448539295</v>
       </c>
       <c r="C281">
         <v>0.01432453135931631</v>
@@ -3485,7 +3485,7 @@
         <v>44294</v>
       </c>
       <c r="B282">
-        <v>0.01463353739951224</v>
+        <v>0.02033739799805506</v>
       </c>
       <c r="C282">
         <v>0.01400122728713172</v>
@@ -3496,7 +3496,7 @@
         <v>44295</v>
       </c>
       <c r="B283">
-        <v>0.01413974615626158</v>
+        <v>0.01981287647430228</v>
       </c>
       <c r="C283">
         <v>0.01372495307107157</v>
@@ -3507,7 +3507,7 @@
         <v>44298</v>
       </c>
       <c r="B284">
-        <v>0.01388546750538148</v>
+        <v>0.01944623072627661</v>
       </c>
       <c r="C284">
         <v>0.01351202312919325</v>
@@ -3518,7 +3518,7 @@
         <v>44299</v>
       </c>
       <c r="B285">
-        <v>0.01359969840680432</v>
+        <v>0.01900772117738775</v>
       </c>
       <c r="C285">
         <v>0.01318310745786744</v>
@@ -3529,7 +3529,7 @@
         <v>44300</v>
       </c>
       <c r="B286">
-        <v>0.01355805683312133</v>
+        <v>0.01887803508655686</v>
       </c>
       <c r="C286">
         <v>0.01293522890633572</v>
@@ -3540,7 +3540,7 @@
         <v>44301</v>
       </c>
       <c r="B287">
-        <v>0.01328167641660047</v>
+        <v>0.0184766989702699</v>
       </c>
       <c r="C287">
         <v>0.0126120907598876</v>
@@ -3551,7 +3551,7 @@
         <v>44302</v>
       </c>
       <c r="B288">
-        <v>0.01298508796597298</v>
+        <v>0.01809635372537452</v>
       </c>
       <c r="C288">
         <v>0.01229707280984771</v>
@@ -3562,7 +3562,7 @@
         <v>44305</v>
       </c>
       <c r="B289">
-        <v>0.01330396974150311</v>
+        <v>0.01867419674648826</v>
       </c>
       <c r="C289">
         <v>0.01200969447158718</v>
@@ -3573,7 +3573,7 @@
         <v>44306</v>
       </c>
       <c r="B290">
-        <v>0.01306865560200076</v>
+        <v>0.01836695904777999</v>
       </c>
       <c r="C290">
         <v>0.01187085219169685</v>
@@ -3584,7 +3584,7 @@
         <v>44308</v>
       </c>
       <c r="B291">
-        <v>0.01282278384597609</v>
+        <v>0.0179927699240098</v>
       </c>
       <c r="C291">
         <v>0.0116744233741737</v>
@@ -3595,7 +3595,7 @@
         <v>44309</v>
       </c>
       <c r="B292">
-        <v>0.01255639882145321</v>
+        <v>0.0176147529735443</v>
       </c>
       <c r="C292">
         <v>0.0115340148429436</v>
@@ -3606,7 +3606,7 @@
         <v>44312</v>
       </c>
       <c r="B293">
-        <v>0.0122819305551686</v>
+        <v>0.01722451179831093</v>
       </c>
       <c r="C293">
         <v>0.01124369181607172</v>
@@ -3617,7 +3617,7 @@
         <v>44313</v>
       </c>
       <c r="B294">
-        <v>0.01240803786076767</v>
+        <v>0.01736603658471165</v>
       </c>
       <c r="C294">
         <v>0.01123984913267388</v>
@@ -3628,7 +3628,7 @@
         <v>44314</v>
       </c>
       <c r="B295">
-        <v>0.0127866036894155</v>
+        <v>0.0178240353496838</v>
       </c>
       <c r="C295">
         <v>0.0113170657915579</v>
@@ -3639,7 +3639,7 @@
         <v>44315</v>
       </c>
       <c r="B296">
-        <v>0.0125899278038779</v>
+        <v>0.01756862053541317</v>
       </c>
       <c r="C296">
         <v>0.01122974961995215</v>
@@ -3650,7 +3650,7 @@
         <v>44316</v>
       </c>
       <c r="B297">
-        <v>0.01252914254555527</v>
+        <v>0.01743964615080017</v>
       </c>
       <c r="C297">
         <v>0.01119573318673119</v>
@@ -3661,7 +3661,7 @@
         <v>44319</v>
       </c>
       <c r="B298">
-        <v>0.01228718385654742</v>
+        <v>0.01710028305903687</v>
       </c>
       <c r="C298">
         <v>0.01092271484917791</v>
@@ -3672,7 +3672,7 @@
         <v>44320</v>
       </c>
       <c r="B299">
-        <v>0.01213093766789958</v>
+        <v>0.01695195835477675</v>
       </c>
       <c r="C299">
         <v>0.01102798268717969</v>
@@ -3683,7 +3683,7 @@
         <v>44321</v>
       </c>
       <c r="B300">
-        <v>0.01237873707371976</v>
+        <v>0.01727285390846966</v>
       </c>
       <c r="C300">
         <v>0.01128079961541472</v>
@@ -3694,7 +3694,7 @@
         <v>44322</v>
       </c>
       <c r="B301">
-        <v>0.01219792378726241</v>
+        <v>0.01706650829920318</v>
       </c>
       <c r="C301">
         <v>0.01100652046343737</v>
@@ -3705,7 +3705,7 @@
         <v>44323</v>
       </c>
       <c r="B302">
-        <v>0.01221105201836139</v>
+        <v>0.01711376886468644</v>
       </c>
       <c r="C302">
         <v>0.01132821650689533</v>
@@ -3716,7 +3716,7 @@
         <v>44326</v>
       </c>
       <c r="B303">
-        <v>0.01201330104993453</v>
+        <v>0.0168381925669642</v>
       </c>
       <c r="C303">
         <v>0.01105699071608573</v>
@@ -3727,7 +3727,7 @@
         <v>44327</v>
       </c>
       <c r="B304">
-        <v>0.01188607856446137</v>
+        <v>0.01667149807738647</v>
       </c>
       <c r="C304">
         <v>0.01088798595172503</v>
@@ -3738,7 +3738,7 @@
         <v>44328</v>
       </c>
       <c r="B305">
-        <v>0.01214424712912318</v>
+        <v>0.0169682515333577</v>
       </c>
       <c r="C305">
         <v>0.0123160679451784</v>
@@ -3749,7 +3749,7 @@
         <v>44329</v>
       </c>
       <c r="B306">
-        <v>0.01200917716480866</v>
+        <v>0.0167964059487826</v>
       </c>
       <c r="C306">
         <v>0.01212587060477532</v>
@@ -3760,7 +3760,7 @@
         <v>44330</v>
       </c>
       <c r="B307">
-        <v>0.0124958002592715</v>
+        <v>0.01743172832458807</v>
       </c>
       <c r="C307">
         <v>0.01197588940896096</v>
@@ -3771,7 +3771,7 @@
         <v>44333</v>
       </c>
       <c r="B308">
-        <v>0.01235118202280581</v>
+        <v>0.01718143056534205</v>
       </c>
       <c r="C308">
         <v>0.01178277185722363</v>
@@ -3782,7 +3782,7 @@
         <v>44334</v>
       </c>
       <c r="B309">
-        <v>0.01211866938132167</v>
+        <v>0.0168578478355129</v>
       </c>
       <c r="C309">
         <v>0.01148785610087814</v>
@@ -3793,7 +3793,7 @@
         <v>44335</v>
       </c>
       <c r="B310">
-        <v>0.01191783187148395</v>
+        <v>0.01666695569698995</v>
       </c>
       <c r="C310">
         <v>0.01123734391749997</v>
@@ -3804,7 +3804,7 @@
         <v>44336</v>
       </c>
       <c r="B311">
-        <v>0.01180062841209029</v>
+        <v>0.01649602617360751</v>
       </c>
       <c r="C311">
         <v>0.0109542555092059</v>
@@ -3815,7 +3815,7 @@
         <v>44337</v>
       </c>
       <c r="B312">
-        <v>0.01216398068099722</v>
+        <v>0.01729914748102136</v>
       </c>
       <c r="C312">
         <v>0.01068759783070794</v>
@@ -3826,7 +3826,7 @@
         <v>44340</v>
       </c>
       <c r="B313">
-        <v>0.01211289982103883</v>
+        <v>0.01711141755346431</v>
       </c>
       <c r="C313">
         <v>0.01066451719618048</v>
@@ -3837,7 +3837,7 @@
         <v>44341</v>
       </c>
       <c r="B314">
-        <v>0.01212145380342341</v>
+        <v>0.01708650664223887</v>
       </c>
       <c r="C314">
         <v>0.01062832652133182</v>
@@ -3848,7 +3848,7 @@
         <v>44342</v>
       </c>
       <c r="B315">
-        <v>0.01194495067495735</v>
+        <v>0.01682471308613304</v>
       </c>
       <c r="C315">
         <v>0.01046761669402756</v>
@@ -3859,7 +3859,7 @@
         <v>44343</v>
       </c>
       <c r="B316">
-        <v>0.01173980939477473</v>
+        <v>0.01652615655523501</v>
       </c>
       <c r="C316">
         <v>0.01020772044065164</v>
@@ -3870,7 +3870,7 @@
         <v>44344</v>
       </c>
       <c r="B317">
-        <v>0.01197334309905114</v>
+        <v>0.01676128045713646</v>
       </c>
       <c r="C317">
         <v>0.01009802808472743</v>
@@ -3881,7 +3881,7 @@
         <v>44347</v>
       </c>
       <c r="B318">
-        <v>0.01175367685526754</v>
+        <v>0.01646366833595223</v>
       </c>
       <c r="C318">
         <v>0.009866650238505179</v>
@@ -3892,7 +3892,7 @@
         <v>44348</v>
       </c>
       <c r="B319">
-        <v>0.01192352489947525</v>
+        <v>0.01678408893796503</v>
       </c>
       <c r="C319">
         <v>0.01008488722664276</v>
@@ -3903,7 +3903,7 @@
         <v>44349</v>
       </c>
       <c r="B320">
-        <v>0.01193861160143025</v>
+        <v>0.01678380738061627</v>
       </c>
       <c r="C320">
         <v>0.009963230006403482</v>
@@ -3914,7 +3914,7 @@
         <v>44351</v>
       </c>
       <c r="B321">
-        <v>0.0118948528875866</v>
+        <v>0.01665274591412368</v>
       </c>
       <c r="C321">
         <v>0.009712470020557112</v>
@@ -3925,7 +3925,7 @@
         <v>44354</v>
       </c>
       <c r="B322">
-        <v>0.01173264148414542</v>
+        <v>0.01639246195328928</v>
       </c>
       <c r="C322">
         <v>0.009473687692891346</v>
@@ -3936,7 +3936,7 @@
         <v>44355</v>
       </c>
       <c r="B323">
-        <v>0.01156505517423238</v>
+        <v>0.01614412557123145</v>
       </c>
       <c r="C323">
         <v>0.009538353563055919</v>
@@ -3947,7 +3947,7 @@
         <v>44356</v>
       </c>
       <c r="B324">
-        <v>0.01133269015756779</v>
+        <v>0.0158229281132736</v>
       </c>
       <c r="C324">
         <v>0.009306120300212203</v>
@@ -3958,7 +3958,7 @@
         <v>44357</v>
       </c>
       <c r="B325">
-        <v>0.01109667608437687</v>
+        <v>0.01549264747200709</v>
       </c>
       <c r="C325">
         <v>0.00907587801433485</v>
@@ -3969,7 +3969,7 @@
         <v>44358</v>
       </c>
       <c r="B326">
-        <v>0.01094182075634372</v>
+        <v>0.015325477890796</v>
       </c>
       <c r="C326">
         <v>0.008998110843278223</v>
@@ -3980,7 +3980,7 @@
         <v>44361</v>
       </c>
       <c r="B327">
-        <v>0.01073088194585544</v>
+        <v>0.01500739248704056</v>
       </c>
       <c r="C327">
         <v>0.008805729284177005</v>
@@ -3991,7 +3991,7 @@
         <v>44362</v>
       </c>
       <c r="B328">
-        <v>0.01059977714612944</v>
+        <v>0.01481178710563488</v>
       </c>
       <c r="C328">
         <v>0.008614058094604971</v>
@@ -4002,7 +4002,7 @@
         <v>44363</v>
       </c>
       <c r="B329">
-        <v>0.0105584097348495</v>
+        <v>0.01471700851683315</v>
       </c>
       <c r="C329">
         <v>0.008608101361966658</v>
@@ -4013,7 +4013,7 @@
         <v>44364</v>
       </c>
       <c r="B330">
-        <v>0.01097370499142445</v>
+        <v>0.01524999987461004</v>
       </c>
       <c r="C330">
         <v>0.008738355674099188</v>
@@ -4024,7 +4024,7 @@
         <v>44365</v>
       </c>
       <c r="B331">
-        <v>0.01085729873961733</v>
+        <v>0.01509673118066375</v>
       </c>
       <c r="C331">
         <v>0.008522646603570874</v>
@@ -4035,7 +4035,7 @@
         <v>44368</v>
       </c>
       <c r="B332">
-        <v>0.01073616115032917</v>
+        <v>0.01489896623215892</v>
       </c>
       <c r="C332">
         <v>0.008386834547930072</v>
@@ -4046,7 +4046,7 @@
         <v>44369</v>
       </c>
       <c r="B333">
-        <v>0.01050921212677597</v>
+        <v>0.01459468703892663</v>
       </c>
       <c r="C333">
         <v>0.00826184360670581</v>
@@ -4057,7 +4057,7 @@
         <v>44370</v>
       </c>
       <c r="B334">
-        <v>0.01024479181608249</v>
+        <v>0.01425166784957101</v>
       </c>
       <c r="C334">
         <v>0.008099691178369769</v>
@@ -4068,7 +4068,7 @@
         <v>44371</v>
       </c>
       <c r="B335">
-        <v>0.01003759601669262</v>
+        <v>0.01395437181200915</v>
       </c>
       <c r="C335">
         <v>0.008051480910696471</v>
@@ -4079,7 +4079,7 @@
         <v>44372</v>
       </c>
       <c r="B336">
-        <v>0.01004872229645506</v>
+        <v>0.01402034967371834</v>
       </c>
       <c r="C336">
         <v>0.008884808454061439</v>
@@ -4090,7 +4090,7 @@
         <v>44375</v>
       </c>
       <c r="B337">
-        <v>0.009874539891110303</v>
+        <v>0.01377379767752223</v>
       </c>
       <c r="C337">
         <v>0.008661542640264875</v>
@@ -4101,7 +4101,7 @@
         <v>44376</v>
       </c>
       <c r="B338">
-        <v>0.009728414072602947</v>
+        <v>0.01356006169902426</v>
       </c>
       <c r="C338">
         <v>0.008447824656411942</v>
@@ -4112,7 +4112,7 @@
         <v>44377</v>
       </c>
       <c r="B339">
-        <v>0.009543233434533203</v>
+        <v>0.01328453452410814</v>
       </c>
       <c r="C339">
         <v>0.008296620940059908</v>
@@ -4123,7 +4123,7 @@
         <v>44378</v>
       </c>
       <c r="B340">
-        <v>0.009460403967240558</v>
+        <v>0.01318013826811028</v>
       </c>
       <c r="C340">
         <v>0.00833696700945747</v>
@@ -4134,7 +4134,7 @@
         <v>44379</v>
       </c>
       <c r="B341">
-        <v>0.009324705285821107</v>
+        <v>0.01298663263966981</v>
       </c>
       <c r="C341">
         <v>0.008808864473098145</v>
@@ -4145,7 +4145,7 @@
         <v>44382</v>
       </c>
       <c r="B342">
-        <v>0.009188459268267829</v>
+        <v>0.01280514450472183</v>
       </c>
       <c r="C342">
         <v>0.008689365745212591</v>
@@ -4156,7 +4156,7 @@
         <v>44383</v>
       </c>
       <c r="B343">
-        <v>0.009589208694750663</v>
+        <v>0.01340315102445112</v>
       </c>
       <c r="C343">
         <v>0.009062603331915461</v>
@@ -4167,7 +4167,7 @@
         <v>44384</v>
       </c>
       <c r="B344">
-        <v>0.009407296229171528</v>
+        <v>0.0131573000667956</v>
       </c>
       <c r="C344">
         <v>0.009471865236246737</v>
@@ -4178,7 +4178,7 @@
         <v>44385</v>
       </c>
       <c r="B345">
-        <v>0.009360729505455804</v>
+        <v>0.01308612938866583</v>
       </c>
       <c r="C345">
         <v>0.009654676786585173</v>
@@ -4189,7 +4189,7 @@
         <v>44389</v>
       </c>
       <c r="B346">
-        <v>0.009267419898092226</v>
+        <v>0.0129378780229256</v>
       </c>
       <c r="C346">
         <v>0.01014650025604941</v>
@@ -4200,7 +4200,7 @@
         <v>44390</v>
       </c>
       <c r="B347">
-        <v>0.00907809471907111</v>
+        <v>0.01265648138323043</v>
       </c>
       <c r="C347">
         <v>0.009926186325595604</v>
@@ -4211,7 +4211,7 @@
         <v>44391</v>
       </c>
       <c r="B348">
-        <v>0.008904210617462159</v>
+        <v>0.0124140965910031</v>
       </c>
       <c r="C348">
         <v>0.009677747833947762</v>
@@ -4222,7 +4222,7 @@
         <v>44392</v>
       </c>
       <c r="B349">
-        <v>0.00883950062289445</v>
+        <v>0.01234603248813814</v>
       </c>
       <c r="C349">
         <v>0.009599303763563197</v>
@@ -4233,7 +4233,7 @@
         <v>44393</v>
       </c>
       <c r="B350">
-        <v>0.008754906992332062</v>
+        <v>0.01225165433481736</v>
       </c>
       <c r="C350">
         <v>0.009734097011511627</v>
@@ -4244,7 +4244,7 @@
         <v>44396</v>
       </c>
       <c r="B351">
-        <v>0.008699729433921916</v>
+        <v>0.01217350527009381</v>
       </c>
       <c r="C351">
         <v>0.009859571606221338</v>
@@ -4255,7 +4255,7 @@
         <v>44397</v>
       </c>
       <c r="B352">
-        <v>0.008670081122418235</v>
+        <v>0.0121496763372178</v>
       </c>
       <c r="C352">
         <v>0.009802178338308588</v>
@@ -4266,7 +4266,7 @@
         <v>44398</v>
       </c>
       <c r="B353">
-        <v>0.008578155641075936</v>
+        <v>0.01201233797748728</v>
       </c>
       <c r="C353">
         <v>0.009605709897417816</v>
@@ -4277,7 +4277,7 @@
         <v>44399</v>
       </c>
       <c r="B354">
-        <v>0.008359495697668003</v>
+        <v>0.01172096396586065</v>
       </c>
       <c r="C354">
         <v>0.009371330068663843</v>
@@ -4288,7 +4288,7 @@
         <v>44400</v>
       </c>
       <c r="B355">
-        <v>0.008214323079658598</v>
+        <v>0.01150932982729801</v>
       </c>
       <c r="C355">
         <v>0.009327261943512686</v>
@@ -4299,7 +4299,7 @@
         <v>44403</v>
       </c>
       <c r="B356">
-        <v>0.008461127766728962</v>
+        <v>0.01183547543288796</v>
       </c>
       <c r="C356">
         <v>0.009258989775081123</v>
@@ -4310,7 +4310,7 @@
         <v>44404</v>
       </c>
       <c r="B357">
-        <v>0.008444281888133207</v>
+        <v>0.01179952216930258</v>
       </c>
       <c r="C357">
         <v>0.009339444746268197</v>
@@ -4321,7 +4321,7 @@
         <v>44405</v>
       </c>
       <c r="B358">
-        <v>0.008678470188938255</v>
+        <v>0.01212188977033564</v>
       </c>
       <c r="C358">
         <v>0.009598719473524402</v>
@@ -4332,7 +4332,7 @@
         <v>44406</v>
       </c>
       <c r="B359">
-        <v>0.008563283238357117</v>
+        <v>0.01195963609081593</v>
       </c>
       <c r="C359">
         <v>0.009416968151375717</v>
@@ -4343,7 +4343,7 @@
         <v>44407</v>
       </c>
       <c r="B360">
-        <v>0.009414269363965867</v>
+        <v>0.01312702329593184</v>
       </c>
       <c r="C360">
         <v>0.011414699456983</v>
@@ -4354,7 +4354,7 @@
         <v>44410</v>
       </c>
       <c r="B361">
-        <v>0.009284488035609283</v>
+        <v>0.01295607945005519</v>
       </c>
       <c r="C361">
         <v>0.01124778915953023</v>
@@ -4365,7 +4365,7 @@
         <v>44411</v>
       </c>
       <c r="B362">
-        <v>0.009372550895300631</v>
+        <v>0.01307073575138082</v>
       </c>
       <c r="C362">
         <v>0.01117645291670998</v>
@@ -4376,7 +4376,7 @@
         <v>44412</v>
       </c>
       <c r="B363">
-        <v>0.009462124501349038</v>
+        <v>0.01320367562986613</v>
       </c>
       <c r="C363">
         <v>0.01129081270355599</v>
@@ -4387,7 +4387,7 @@
         <v>44413</v>
       </c>
       <c r="B364">
-        <v>0.01129756474694812</v>
+        <v>0.01573867141334011</v>
       </c>
       <c r="C364">
         <v>0.01100497413766701</v>
@@ -4398,7 +4398,7 @@
         <v>44414</v>
       </c>
       <c r="B365">
-        <v>0.01106886203981782</v>
+        <v>0.01543389319776886</v>
       </c>
       <c r="C365">
         <v>0.01099847284430896</v>
@@ -4409,7 +4409,7 @@
         <v>44417</v>
       </c>
       <c r="B366">
-        <v>0.01082848157159907</v>
+        <v>0.01510331069555015</v>
       </c>
       <c r="C366">
         <v>0.01073575711627229</v>
@@ -4420,7 +4420,7 @@
         <v>44418</v>
       </c>
       <c r="B367">
-        <v>0.01061422443254644</v>
+        <v>0.01481518089723459</v>
       </c>
       <c r="C367">
         <v>0.0105407347172572</v>
@@ -4431,7 +4431,7 @@
         <v>44419</v>
       </c>
       <c r="B368">
-        <v>0.01041119968460092</v>
+        <v>0.01453627306810863</v>
       </c>
       <c r="C368">
         <v>0.01027384828578197</v>
@@ -4442,7 +4442,7 @@
         <v>44420</v>
       </c>
       <c r="B369">
-        <v>0.01034682115613375</v>
+        <v>0.01442419087174482</v>
       </c>
       <c r="C369">
         <v>0.01024969068747341</v>
@@ -4453,7 +4453,7 @@
         <v>44421</v>
       </c>
       <c r="B370">
-        <v>0.01018803670158562</v>
+        <v>0.01416942456547064</v>
       </c>
       <c r="C370">
         <v>0.0100673201522784</v>
@@ -4464,7 +4464,7 @@
         <v>44424</v>
       </c>
       <c r="B371">
-        <v>0.01022765242493005</v>
+        <v>0.01422338002139521</v>
       </c>
       <c r="C371">
         <v>0.01037134986886403</v>
@@ -4475,7 +4475,7 @@
         <v>44425</v>
       </c>
       <c r="B372">
-        <v>0.01004733729981491</v>
+        <v>0.01395804909077472</v>
       </c>
       <c r="C372">
         <v>0.01028292135172562</v>
@@ -4486,7 +4486,7 @@
         <v>44426</v>
       </c>
       <c r="B373">
-        <v>0.01000798077453371</v>
+        <v>0.01388446542762265</v>
       </c>
       <c r="C373">
         <v>0.01018077181241468</v>
@@ -4497,7 +4497,7 @@
         <v>44427</v>
       </c>
       <c r="B374">
-        <v>0.01018807814733306</v>
+        <v>0.01417874354785212</v>
       </c>
       <c r="C374">
         <v>0.01005406410081084</v>
@@ -4508,7 +4508,7 @@
         <v>44428</v>
       </c>
       <c r="B375">
-        <v>0.009927853430658329</v>
+        <v>0.01382828474351874</v>
       </c>
       <c r="C375">
         <v>0.01004553183307825</v>
@@ -4519,7 +4519,7 @@
         <v>44431</v>
       </c>
       <c r="B376">
-        <v>0.009832125222205225</v>
+        <v>0.0136774179428601</v>
       </c>
       <c r="C376">
         <v>0.009810888269496588</v>
@@ -4530,7 +4530,7 @@
         <v>44432</v>
       </c>
       <c r="B377">
-        <v>0.01006879626167475</v>
+        <v>0.01400446600856515</v>
       </c>
       <c r="C377">
         <v>0.01103535144582354</v>
@@ -4541,7 +4541,7 @@
         <v>44433</v>
       </c>
       <c r="B378">
-        <v>0.009799670832630626</v>
+        <v>0.0136453821103948</v>
       </c>
       <c r="C378">
         <v>0.01083505238445516</v>
@@ -4552,7 +4552,7 @@
         <v>44434</v>
       </c>
       <c r="B379">
-        <v>0.009713139941361342</v>
+        <v>0.01349979907379951</v>
       </c>
       <c r="C379">
         <v>0.01117909337307574</v>
@@ -4563,7 +4563,7 @@
         <v>44435</v>
       </c>
       <c r="B380">
-        <v>0.01011834508793794</v>
+        <v>0.01400179412279663</v>
       </c>
       <c r="C380">
         <v>0.01156794799946109</v>
@@ -4574,7 +4574,7 @@
         <v>44438</v>
       </c>
       <c r="B381">
-        <v>0.009917166648651232</v>
+        <v>0.01372601574201315</v>
       </c>
       <c r="C381">
         <v>0.01138349759754281</v>
@@ -4585,7 +4585,7 @@
         <v>44439</v>
       </c>
       <c r="B382">
-        <v>0.0102587776836425</v>
+        <v>0.0142335864045583</v>
       </c>
       <c r="C382">
         <v>0.0112017841784963</v>
@@ -4596,7 +4596,7 @@
         <v>44440</v>
       </c>
       <c r="B383">
-        <v>0.01003160835936661</v>
+        <v>0.01394529979508491</v>
       </c>
       <c r="C383">
         <v>0.01100932795441842</v>
@@ -4607,7 +4607,7 @@
         <v>44441</v>
       </c>
       <c r="B384">
-        <v>0.01009290874316917</v>
+        <v>0.01401113123311098</v>
       </c>
       <c r="C384">
         <v>0.01175638906910712</v>
@@ -4618,7 +4618,7 @@
         <v>44442</v>
       </c>
       <c r="B385">
-        <v>0.009836811654512417</v>
+        <v>0.01369163223579352</v>
       </c>
       <c r="C385">
         <v>0.01149684048126236</v>
@@ -4629,7 +4629,7 @@
         <v>44445</v>
       </c>
       <c r="B386">
-        <v>0.009642072221891226</v>
+        <v>0.0134329263321427</v>
       </c>
       <c r="C386">
         <v>0.01140988814430911</v>
@@ -4640,7 +4640,7 @@
         <v>44447</v>
       </c>
       <c r="B387">
-        <v>0.01081098126121766</v>
+        <v>0.01506611307450649</v>
       </c>
       <c r="C387">
         <v>0.0137554474072521</v>
@@ -4651,7 +4651,7 @@
         <v>44448</v>
       </c>
       <c r="B388">
-        <v>0.0107873016289972</v>
+        <v>0.01501731865212954</v>
       </c>
       <c r="C388">
         <v>0.01411698533978962</v>
@@ -4662,7 +4662,7 @@
         <v>44449</v>
       </c>
       <c r="B389">
-        <v>0.01056076849760523</v>
+        <v>0.01472532640868493</v>
       </c>
       <c r="C389">
         <v>0.01384689991613027</v>
@@ -4673,7 +4673,7 @@
         <v>44452</v>
       </c>
       <c r="B390">
-        <v>0.0108139190069411</v>
+        <v>0.01506830085975424</v>
       </c>
       <c r="C390">
         <v>0.0142481226850308</v>
@@ -4684,7 +4684,7 @@
         <v>44453</v>
       </c>
       <c r="B391">
-        <v>0.01062310176104626</v>
+        <v>0.01482080547566739</v>
       </c>
       <c r="C391">
         <v>0.01388758945090122</v>
@@ -4695,7 +4695,7 @@
         <v>44454</v>
       </c>
       <c r="B392">
-        <v>0.01060662220561813</v>
+        <v>0.0147554080375285</v>
       </c>
       <c r="C392">
         <v>0.01365074458676124</v>
@@ -4706,7 +4706,7 @@
         <v>44455</v>
       </c>
       <c r="B393">
-        <v>0.01061226961648461</v>
+        <v>0.01471591579168948</v>
       </c>
       <c r="C393">
         <v>0.01345278201429163</v>
@@ -4717,7 +4717,7 @@
         <v>44456</v>
       </c>
       <c r="B394">
-        <v>0.01108335757668042</v>
+        <v>0.01538059894046645</v>
       </c>
       <c r="C394">
         <v>0.01371725908582495</v>
@@ -4728,7 +4728,7 @@
         <v>44459</v>
       </c>
       <c r="B395">
-        <v>0.01105287438282786</v>
+        <v>0.01531250896583499</v>
       </c>
       <c r="C395">
         <v>0.0140769490082664</v>
@@ -4739,7 +4739,7 @@
         <v>44460</v>
       </c>
       <c r="B396">
-        <v>0.01112741902064</v>
+        <v>0.01540071337282768</v>
       </c>
       <c r="C396">
         <v>0.0142229571217348</v>

</xml_diff>